<commit_message>
240705 Fixing u & v calculation
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cuong\Project\Transportation Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4C32CB-475A-4FDF-956E-AE1AD2FAAE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2A723-5FF1-4E19-AE65-6C6EE51CEE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACD73CE0-681C-457A-BD40-66717F83DA7A}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,7 +426,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -514,7 +510,7 @@
         <v>300</v>
       </c>
       <c r="D5" s="2">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E5" s="5"/>
     </row>

</xml_diff>

<commit_message>
250705 Update Input and Output in tkinter
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cuong\Project\Transportation Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2A723-5FF1-4E19-AE65-6C6EE51CEE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8BB322-5B91-46F4-9817-5BE46783E20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACD73CE0-681C-457A-BD40-66717F83DA7A}"/>
   </bookViews>
@@ -36,33 +36,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -70,45 +52,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,96 +372,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C50070-284E-4535-A500-45DB528442C0}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3">
-        <v>7</v>
-      </c>
-      <c r="E1" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f ca="1">ROUND(RAND()*100,2)</f>
+        <v>72.849999999999994</v>
+      </c>
+      <c r="B1">
+        <f t="shared" ref="B1:G1" ca="1" si="0">ROUND(RAND()*100,2)</f>
+        <v>91.34</v>
+      </c>
+      <c r="C1">
+        <f t="shared" ca="1" si="0"/>
+        <v>61.17</v>
+      </c>
+      <c r="D1">
+        <f t="shared" ca="1" si="0"/>
+        <v>99.68</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ca="1" si="0"/>
+        <v>36.04</v>
+      </c>
+      <c r="F1">
+        <f t="shared" ca="1" si="0"/>
+        <v>56.78</v>
+      </c>
+      <c r="G1">
+        <f t="shared" ca="1" si="0"/>
+        <v>79.17</v>
+      </c>
+      <c r="H1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f t="shared" ref="A2:G10" ca="1" si="1">ROUND(RAND()*100,2)</f>
+        <v>28.89</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ca="1" si="1"/>
+        <v>68.319999999999993</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ca="1" si="1"/>
+        <v>18.940000000000001</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ca="1" si="1"/>
+        <v>80.36</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ca="1" si="1"/>
+        <v>57.97</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="1"/>
+        <v>33.72</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="1"/>
+        <v>66.8</v>
+      </c>
+      <c r="H2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.14</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="1"/>
+        <v>78.16</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="1"/>
+        <v>12.2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="1"/>
+        <v>86.14</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="1"/>
+        <v>82.6</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="1"/>
+        <v>84.28</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="1"/>
+        <v>61.3</v>
+      </c>
+      <c r="H3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="1"/>
+        <v>92.33</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="1"/>
+        <v>35.869999999999997</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>34.72</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>33.04</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="1"/>
+        <v>11.95</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30.09</v>
+      </c>
+      <c r="H4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.16</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.45</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.08</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>30.61</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>21.5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="1"/>
+        <v>29.97</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="1"/>
+        <v>46.25</v>
+      </c>
+      <c r="H5">
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>53.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="1"/>
+        <v>61.14</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="1"/>
+        <v>91.33</v>
+      </c>
+      <c r="H6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="1"/>
+        <v>68.819999999999993</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>86.72</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>73.64</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.83</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>36.32</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="1"/>
+        <v>32.19</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="1"/>
+        <v>80.95</v>
+      </c>
+      <c r="H7">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.98</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="1"/>
+        <v>78.650000000000006</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>12.2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>16.23</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="1"/>
+        <v>78.09</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.97</v>
+      </c>
+      <c r="H8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="1"/>
+        <v>88.98</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>68.61</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="1"/>
+        <v>19.829999999999998</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>40.659999999999997</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>56.9</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="1"/>
+        <v>30.53</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="1"/>
+        <v>60.85</v>
+      </c>
+      <c r="H9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.87</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="1"/>
+        <v>75.11</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="1"/>
+        <v>47.15</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>88.32</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>15.15</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="1"/>
+        <v>98.26</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="1"/>
+        <v>61.91</v>
+      </c>
+      <c r="H10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>400</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>150</v>
-      </c>
-      <c r="B5" s="2">
-        <v>200</v>
-      </c>
-      <c r="C5" s="2">
-        <v>300</v>
-      </c>
-      <c r="D5" s="2">
-        <v>500</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="B11">
+        <v>600</v>
+      </c>
+      <c r="C11">
+        <v>230</v>
+      </c>
+      <c r="D11">
+        <v>120</v>
+      </c>
+      <c r="E11">
+        <v>650</v>
+      </c>
+      <c r="F11">
+        <v>230</v>
+      </c>
+      <c r="G11">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>